<commit_message>
adding kris' python notebook
</commit_message>
<xml_diff>
--- a/nbadata2950.xlsx
+++ b/nbadata2950.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sachinshah/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishanweber/Documents/github/info2950project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A2462E-A48B-2745-B21F-5ADD2E22620C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D33ADC2F-F18E-9949-AE14-2A391CAFC79C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15840" activeTab="7" xr2:uid="{CF221EA7-8924-2D4F-BF2C-6192ED554EEE}"/>
   </bookViews>
@@ -318,8 +318,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10783,88 +10783,88 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>61</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="5"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -12728,11 +12728,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -12740,12 +12741,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://stats.nba.com/team/1610612749/traditional/?" xr:uid="{BBA2DF3A-24BC-254A-BDA2-062A0516058E}"/>
@@ -12794,88 +12794,88 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>61</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="5"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -13871,11 +13871,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -13883,12 +13884,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://stats.nba.com/team/1610612761/traditional/?" xr:uid="{0ECE5BCA-3FB5-F24C-8C19-20DD6A60F1CD}"/>
@@ -13923,88 +13923,88 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -15000,6 +15000,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
@@ -15007,18 +15019,6 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://stats.nba.com/team/1610612747/traditional/?" xr:uid="{71C6B8D9-4641-184A-8FD9-6EB4A7EC4350}"/>

</xml_diff>